<commit_message>
Changed met data title
</commit_message>
<xml_diff>
--- a/meta-data/surface-met-metadata.xlsx
+++ b/meta-data/surface-met-metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heather/Desktop/AOM-WP1-BL/meta-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{649AFB05-DCA1-474D-A6C3-ECA1FCDBC5EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA23DA1-77A7-9340-A14D-3FD5FABDE095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23220" windowHeight="19780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -211,9 +211,6 @@
     <t>1</t>
   </si>
   <si>
-    <t>Ice Station surface met data</t>
-  </si>
-  <si>
     <t>sonic anemometer - Metek,
 gas analyser - LI-COR, 
 temperature/humidity sensor - Vaisala, 
@@ -261,6 +258,9 @@
 (6) The Met mast KT15 (skin_temperature_1) had an window heater activated. The radiometer stand KT15 (skin_temperature_2) did not.
 (7) The factory calibration is used for the heat-flux plate data.
 (8) 1-minute averages are labelled for the LHS of the averaging window. </t>
+  </si>
+  <si>
+    <t>Ice Station surface meteorology and radiation data</t>
   </si>
 </sst>
 </file>
@@ -697,7 +697,7 @@
   <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="B37" sqref="B37"/>
@@ -739,7 +739,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -747,7 +747,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -755,7 +755,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -819,7 +819,7 @@
         <v>58</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -937,7 +937,7 @@
         <v>31</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -998,7 +998,7 @@
         <v>38</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -1006,7 +1006,7 @@
         <v>39</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added KT15 bias correction
</commit_message>
<xml_diff>
--- a/meta-data/surface-met-metadata.xlsx
+++ b/meta-data/surface-met-metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heather/Desktop/AOM-WP1-BL/meta-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943CEE6B-214F-A848-8964-B35C209F0680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FED97B2-F943-9142-AC81-E5EFE454BEC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23220" windowHeight="19780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14420" yWindow="500" windowWidth="23220" windowHeight="19780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="global-attributes" sheetId="1" r:id="rId1"/>
@@ -247,20 +247,20 @@
 snow thermistors - N/A</t>
   </si>
   <si>
+    <t>Ice Station surface meteorology and radiation data</t>
+  </si>
+  <si>
+    <t>2 m a.s.l</t>
+  </si>
+  <si>
     <t xml:space="preserve">(1) The radiometer stand (all hemispheric radiosometers and the KT15-2) was located approximately 40 m away from the met mast (all other instruments).
 (2) True wind directions are calculated using the heading between the two GPS units on the Met Mast and the radiometer stand. 
 (3) Vector wind averages are calculated before derving the True wind direction in degrees.
 (4) No tilt correction is applied to the 3D sonic anemometer data. Horizontal wind speed is calculated from all 3D componenets, assuming that the contribution of vertical velocity is negligible.  
 (5) Air pressure in this file is derived from the internal sensor in the Licor control box, no corrections have been applied. 
-(6) The Met mast KT15 (skin_temperature_1) had an window heater activated. The radiometer stand KT15 (skin_temperature_2) did not.
+(6) A bias correction has been applied to the Met mast KT15 (skin_temperature_1) based on the recorded temperature of melting snow. The instrument bias is due to the winsow heater that was activated on the Met mast KT15. 
 (7) The factory calibration is used for the heat-flux plate data.
 (8) 1-minute averages are labelled for the LHS of the averaging window. </t>
-  </si>
-  <si>
-    <t>Ice Station surface meteorology and radiation data</t>
-  </si>
-  <si>
-    <t>2 m a.s.l</t>
   </si>
 </sst>
 </file>
@@ -697,10 +697,10 @@
   <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B34" sqref="B34"/>
+      <selection pane="bottomRight" activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -937,7 +937,7 @@
         <v>31</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -982,7 +982,7 @@
         <v>36</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1006,7 +1006,7 @@
         <v>39</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>